<commit_message>
Transaksi dicky branch (#38)
* read excel done

* done add

* new transakciton

* pemanasan global

* new

* new

* pp

* gacor transkasi

* validasi baru

* curr

* new

* new

* done separator sisa edit

* done separator

* lock unlcok

* new bug

* Test

* new

* ppp

* ppp

* View mo ppc done

* pppp

* srug

* sds

* gacorrr

* ambatunat

* pppp

* ppp

* jomok 1

* kelass

* asa

* newst

* nnn

* new-add-ppc clear

* nothing

* new

* fix 1

* amba fix

* new batik

* new

* pp

* ppp

* new rev validate total v1

* Doneee

* ppp

* aa

* pp

* pp

* pp

* new

* ea mabar skuy living goat

* gacor

* kakka

* new

* new pus

* newer

* fxing bugss

* ahahha

* PPP

* pp

* newer

* newerrr
</commit_message>
<xml_diff>
--- a/src/assets/Template Excel/Layout_Plant.xlsx
+++ b/src/assets/Template Excel/Layout_Plant.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJEK SRI\TEMPLATE EXCEL\New Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkTools SRI\Frontend\sri_monthly_planning_fe\src\assets\Template Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FCFC9C-1ABB-4491-A28F-AD2DD0B37C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5FFE96-62D3-40A3-A7CC-65610522616A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6DA0EC4C-990A-47CA-B09E-B24038995E24}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{6DA0EC4C-990A-47CA-B09E-B24038995E24}"/>
   </bookViews>
   <sheets>
     <sheet name="PLANT" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,37 +36,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>PLANT_ID</t>
   </si>
   <si>
     <t>PLANT_NAME</t>
   </si>
+  <si>
+    <t>NOMOR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -79,6 +65,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -95,7 +86,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -118,26 +109,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -157,9 +173,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -197,7 +213,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -303,7 +319,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -445,7 +461,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -453,65 +469,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B6DA4D-E0D7-490B-9821-AEDE834B2E5C}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>